<commit_message>
CHANGED: updating the xlsx template for feature registration.
</commit_message>
<xml_diff>
--- a/find_artek/static_root/publications/docs/find-artek_feature_registration.xlsx
+++ b/find_artek/static_root/publications/docs/find-artek_feature_registration.xlsx
@@ -66,7 +66,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Feature identifier used to determine if geometries are to be added to the same or a new feature object. One feature may consist of several points f.ex. - in which case the Feature#-column should hold the same value for all geometries. Non-geometry fields (e.g. name, description etc. is read from the first row reffering to a specific feature#.</t>
+Feature identifier used to determine if geometries are to be added to the same or a new feature object. A line feature, f.ex. consists of several points - in which case the Feature#-column should hold the same value for all the rows that are to be added to the same line feature. The rows will be added to the line/polygon in the order they occur in the sheet. The feature type and srid must be the same in all rows that are to be added to the same line/polygon. 
+Non-geometry fields (e.g. name, description etc.) is read from the first row reffering to a specific feature#.</t>
         </r>
       </text>
     </comment>
@@ -114,7 +115,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose from drop down list (only geometry type "point" supported.</t>
+Choose from drop down list (point, line or polygon)</t>
         </r>
       </text>
     </comment>
@@ -138,7 +139,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Choose as appropriate from drop down list</t>
+Choose the appropriate spatial reference id (srid) from the drop down list.
+The srid depends on how the coordinates were obtained and processed.</t>
         </r>
       </text>
     </comment>
@@ -252,16 +254,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Thomas Ingeman-Nielsen:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Thomas Ingeman-Nielsen:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A meaningful textual description of the feature. Could include information on what measurements or observations were obtained, main results, etc.
 Use ALT+ENTER to make a line break inside a cell.</t>
         </r>
       </text>
@@ -286,7 +289,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mainly used for images, the direction in which the image was taken.</t>
+Mainly used for images: the cardinal direction (N, S, E, W, SE, NW, etc.) in which the image was taken.</t>
         </r>
       </text>
     </comment>
@@ -573,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -608,9 +611,6 @@
     <t>Geometry_type</t>
   </si>
   <si>
-    <t>WGS84 Lon/Lat</t>
-  </si>
-  <si>
     <t>WGS 84 / UTM zone 22N</t>
   </si>
   <si>
@@ -642,9 +642,6 @@
   </si>
   <si>
     <t>SRID code</t>
-  </si>
-  <si>
-    <t>Global projection</t>
   </si>
   <si>
     <t>Most of West Greenland covered</t>
@@ -727,6 +724,57 @@
   </si>
   <si>
     <t>Thule / Qaanaaq area</t>
+  </si>
+  <si>
+    <t>WGS84 Longitude/Latitude</t>
+  </si>
+  <si>
+    <t>Global system, geographical coordinates</t>
+  </si>
+  <si>
+    <t>txt_code</t>
+  </si>
+  <si>
+    <t>utm22_gr96</t>
+  </si>
+  <si>
+    <t>geo_wgs84</t>
+  </si>
+  <si>
+    <t>utm18_wgs84</t>
+  </si>
+  <si>
+    <t>utm19_wgs84</t>
+  </si>
+  <si>
+    <t>utm20_wgs84</t>
+  </si>
+  <si>
+    <t>utm21_wgs84</t>
+  </si>
+  <si>
+    <t>utm22_wgs84</t>
+  </si>
+  <si>
+    <t>utm23_wgs84</t>
+  </si>
+  <si>
+    <t>utm24_wgs84</t>
+  </si>
+  <si>
+    <t>utm25_wgs84</t>
+  </si>
+  <si>
+    <t>utm26_wgs84</t>
+  </si>
+  <si>
+    <t>utm27_wgs84</t>
+  </si>
+  <si>
+    <t>utm28_wgs84</t>
+  </si>
+  <si>
+    <t>utm29_wgs84</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1211,7 @@
   <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1221,7 @@
     <col min="3" max="3" width="15.7109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14" style="11" customWidth="1"/>
     <col min="7" max="8" width="15.85546875" style="11" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" style="11" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="12" customWidth="1"/>
@@ -1185,7 +1233,7 @@
   <sheetData>
     <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -1209,7 +1257,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -1291,8 +1339,8 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="3"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
@@ -2478,18 +2526,18 @@
       <c r="T78"/>
     </row>
   </sheetData>
-  <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>"point"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"GEOPHYSICAL DATA,FIELD MEASUREMENT,RESOURCE,PHOTO,SAMPLE,OTHER,BOREHOLE,LAB MEASUREMENT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="The field value must be taken from the list of choices." sqref="I2:I1048576">
       <formula1>"Approximate, GPS (phase), GPS (code), Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"point,line,polygon"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>COUNTIF($B:$B,B1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
@@ -2513,34 +2561,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="C1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2548,13 +2600,16 @@
         <v>3182</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2562,13 +2617,16 @@
         <v>4326</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2576,11 +2634,14 @@
         <v>32618</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2588,13 +2649,16 @@
         <v>32619</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2602,11 +2666,14 @@
         <v>32620</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2614,13 +2681,16 @@
         <v>32621</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2628,13 +2698,16 @@
         <v>32622</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2642,13 +2715,16 @@
         <v>32623</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2656,13 +2732,16 @@
         <v>32624</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2670,13 +2749,16 @@
         <v>32625</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2684,13 +2766,16 @@
         <v>32626</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2698,13 +2783,16 @@
         <v>32627</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2712,13 +2800,16 @@
         <v>32628</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2726,74 +2817,84 @@
         <v>32629</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
     </row>
   </sheetData>
   <sortState ref="A2:D24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2804,7 +2905,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,13 +2919,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="2"/>
       <c r="E1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2832,89 +2933,71 @@
       <c r="I1" s="7"/>
       <c r="J1" s="2"/>
       <c r="K1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="7"/>
       <c r="J2" s="2"/>
       <c r="K2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="10">
-        <f>A3+B3/60+C3/3600</f>
+        <f>IF(A3&gt;=0,A3+B3/60+C3/3600,A3-B3/60-C3/3600)</f>
         <v>0</v>
       </c>
       <c r="L3" s="10">
-        <f>E3+F3/60+G3/3600</f>
+        <f>IF(E3&gt;=0,E3+F3/60+G3/3600,E3-F3/60-G3/3600)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="10">
-        <f t="shared" ref="K4:K23" si="0">A4+B4/60+C4/3600</f>
+        <f t="shared" ref="K4:K23" si="0">IF(A4&gt;=0,A4+B4/60+C4/3600,A4-B4/60-C4/3600)</f>
         <v>0</v>
       </c>
       <c r="L4" s="10">
-        <f t="shared" ref="L4:L23" si="1">E4+F4/60+G4/3600</f>
+        <f t="shared" ref="L4:L23" si="1">IF(E4&gt;=0,E4+F4/60+G4/3600,E4-F4/60-G4/3600)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" si="0"/>
@@ -2927,7 +3010,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="10">
         <f t="shared" si="0"/>
@@ -2940,7 +3023,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="10">
         <f t="shared" si="0"/>
@@ -2953,7 +3036,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" s="10">
         <f t="shared" si="0"/>
@@ -2966,7 +3049,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="10">
         <f t="shared" si="0"/>
@@ -2979,7 +3062,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" s="10">
         <f t="shared" si="0"/>
@@ -2992,7 +3075,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" s="10">
         <f t="shared" si="0"/>
@@ -3005,7 +3088,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K12" s="10">
         <f t="shared" si="0"/>
@@ -3018,7 +3101,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="0"/>
@@ -3031,7 +3114,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" s="10">
         <f t="shared" si="0"/>
@@ -3044,7 +3127,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" s="10">
         <f t="shared" si="0"/>
@@ -3057,7 +3140,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="0"/>
@@ -3070,7 +3153,7 @@
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="0"/>
@@ -3083,7 +3166,7 @@
     </row>
     <row r="18" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K18" s="10">
         <f t="shared" si="0"/>
@@ -3096,7 +3179,7 @@
     </row>
     <row r="19" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19" s="10">
         <f t="shared" si="0"/>
@@ -3109,7 +3192,7 @@
     </row>
     <row r="20" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I20" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K20" s="10">
         <f t="shared" si="0"/>
@@ -3122,7 +3205,7 @@
     </row>
     <row r="21" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K21" s="10">
         <f t="shared" si="0"/>
@@ -3135,7 +3218,7 @@
     </row>
     <row r="22" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K22" s="10">
         <f t="shared" si="0"/>
@@ -3148,7 +3231,7 @@
     </row>
     <row r="23" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I23" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" s="10">
         <f t="shared" si="0"/>
@@ -3191,7 +3274,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -3215,7 +3298,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -3238,13 +3321,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3">
         <v>32622</v>
@@ -3256,13 +3339,13 @@
         <v>7427269.1699999999</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" s="4">
         <v>41336</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -3275,13 +3358,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3">
         <v>4326</v>
@@ -3293,13 +3376,13 @@
         <v>66.940393869999994</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4">
         <v>41336</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>

</xml_diff>